<commit_message>
throw an error if a cell value cannot be converted to a numeric value EF-4206
</commit_message>
<xml_diff>
--- a/datatable/testfiles/liste.xlsx
+++ b/datatable/testfiles/liste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caspari\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\roXtraRepos\services\datatable\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E326C71-9FAA-42B4-839F-4C2183883C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD26D108-EB72-41FA-BFA4-C8E269A95A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="38610" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38295" yWindow="0" windowWidth="38610" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Adresse</t>
   </si>
@@ -45,9 +45,6 @@
     <t>+49 30 1234567</t>
   </si>
   <si>
-    <t>TS-001</t>
-  </si>
-  <si>
     <t>Green Energy Inc.</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>+49 89 9876543</t>
   </si>
   <si>
-    <t>GE-002</t>
-  </si>
-  <si>
     <t>Creative Minds Agency</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>+49 211 5678901</t>
   </si>
   <si>
-    <t>CMA-003</t>
-  </si>
-  <si>
     <t>Finance Experts Ltd.</t>
   </si>
   <si>
@@ -81,9 +72,6 @@
     <t>+49 40 2345678</t>
   </si>
   <si>
-    <t>FE-004</t>
-  </si>
-  <si>
     <t>Digital Innovations</t>
   </si>
   <si>
@@ -93,9 +81,6 @@
     <t>+49 511 3456789</t>
   </si>
   <si>
-    <t>DI-005</t>
-  </si>
-  <si>
     <t>Health Dynamics</t>
   </si>
   <si>
@@ -105,9 +90,6 @@
     <t>+49 221 4567890</t>
   </si>
   <si>
-    <t>HD-006</t>
-  </si>
-  <si>
     <t>Global Connections</t>
   </si>
   <si>
@@ -117,9 +99,6 @@
     <t>+49 69 6789012</t>
   </si>
   <si>
-    <t>GC-007</t>
-  </si>
-  <si>
     <t>Smart Solutions Inc.</t>
   </si>
   <si>
@@ -129,9 +108,6 @@
     <t>+49 711 7890123</t>
   </si>
   <si>
-    <t>SSI-008</t>
-  </si>
-  <si>
     <t>Future Technologies</t>
   </si>
   <si>
@@ -141,9 +117,6 @@
     <t>+49 911 8901234</t>
   </si>
   <si>
-    <t>FT-009</t>
-  </si>
-  <si>
     <t>Web Development Ltd.</t>
   </si>
   <si>
@@ -153,9 +126,6 @@
     <t>+49 89 0123456</t>
   </si>
   <si>
-    <t>WD-010</t>
-  </si>
-  <si>
     <t>Data Analytics Group</t>
   </si>
   <si>
@@ -165,9 +135,6 @@
     <t>+49 69 1234567</t>
   </si>
   <si>
-    <t>DAG-011</t>
-  </si>
-  <si>
     <t>Media Productions</t>
   </si>
   <si>
@@ -177,9 +144,6 @@
     <t>+49 211 2345678</t>
   </si>
   <si>
-    <t>MP-012</t>
-  </si>
-  <si>
     <t>Design Studio GmbH</t>
   </si>
   <si>
@@ -189,9 +153,6 @@
     <t>+49 30 3456789</t>
   </si>
   <si>
-    <t>DS-013</t>
-  </si>
-  <si>
     <t>International Trade</t>
   </si>
   <si>
@@ -201,45 +162,30 @@
     <t>+49 40 4567890</t>
   </si>
   <si>
-    <t>IT-014</t>
-  </si>
-  <si>
     <t>Legal Consultancy</t>
   </si>
   <si>
     <t>Wilhelmstraße 567, 40215 Düsseldorf</t>
   </si>
   <si>
-    <t>LC-015</t>
-  </si>
-  <si>
     <t>Energy Solutions</t>
   </si>
   <si>
     <t>Königsallee 12, 60313 Frankfurt am Main</t>
   </si>
   <si>
-    <t>ES-016</t>
-  </si>
-  <si>
     <t>Software Innovations</t>
   </si>
   <si>
     <t>Marktallee 678, 70182 Stuttgart</t>
   </si>
   <si>
-    <t>SI-017</t>
-  </si>
-  <si>
     <t>Research Institute</t>
   </si>
   <si>
     <t>Goethestraße 34, 80538 München</t>
   </si>
   <si>
-    <t>RI-018</t>
-  </si>
-  <si>
     <t>Marketing Agency</t>
   </si>
   <si>
@@ -249,9 +195,6 @@
     <t>+49 221 1234567</t>
   </si>
   <si>
-    <t>MA-019</t>
-  </si>
-  <si>
     <t>Real Estate Group</t>
   </si>
   <si>
@@ -259,9 +202,6 @@
   </si>
   <si>
     <t>+49 30 2345678</t>
-  </si>
-  <si>
-    <t>REG-020</t>
   </si>
   <si>
     <t>Name</t>
@@ -667,7 +607,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +620,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -692,7 +632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -702,277 +642,278 @@
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="4">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="4">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="4">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="D5" s="4">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D7" s="4">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="D8" s="4">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="D9" s="4">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D10" s="4">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D11" s="4">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="D12" s="4">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="D13" s="4">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D14" s="4">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D15" s="4">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="C18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="D20" s="4">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>78</v>
+      <c r="D21" s="4">
+        <v>1020</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>